<commit_message>
Grouping of files and deletion of unnecessary files
Grouping of files for the connection in a different folder
</commit_message>
<xml_diff>
--- a/projectProgress/devPlanning.xlsx
+++ b/projectProgress/devPlanning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sifaka\AndroidStudioProjects\Mediatheque\projectProgress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60FA7EF9-B43B-4E90-96E4-876D60251C7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC628A7B-E8AF-4884-976C-1E2531B96867}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5CEC0A7F-10D1-4F8B-A673-19C9D4440BAD}"/>
   </bookViews>
@@ -63,9 +63,6 @@
     <t>Semaine 12</t>
   </si>
   <si>
-    <t>Débogage et finalisation</t>
-  </si>
-  <si>
     <t>Pouvoir modifier une entré en base</t>
   </si>
   <si>
@@ -78,9 +75,6 @@
     <t>Pouvoir naviguer entre les différentes rubriques</t>
   </si>
   <si>
-    <t>Regarder se qui se fait déjà sur le google play</t>
-  </si>
-  <si>
     <t>Prise en main de Firebase Firestore &amp; Auth</t>
   </si>
   <si>
@@ -91,6 +85,12 @@
   </si>
   <si>
     <t>Temps mis réellement</t>
+  </si>
+  <si>
+    <t>Test et finalisation</t>
+  </si>
+  <si>
+    <t>Étude de l'existant -&gt; étude comparative -&gt; veille technologique</t>
   </si>
 </sst>
 </file>
@@ -246,9 +246,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="15" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -286,6 +283,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -616,376 +616,374 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{865E9418-04D3-482C-83C1-D6C6486673AD}">
   <dimension ref="A1:CE22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="53" customWidth="1"/>
+    <col min="1" max="1" width="57.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:83" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6" t="s">
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6" t="s">
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
-      <c r="W1" s="6" t="s">
+      <c r="Q1" s="19"/>
+      <c r="R1" s="19"/>
+      <c r="S1" s="19"/>
+      <c r="T1" s="19"/>
+      <c r="U1" s="19"/>
+      <c r="V1" s="19"/>
+      <c r="W1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="X1" s="6"/>
-      <c r="Y1" s="6"/>
-      <c r="Z1" s="6"/>
-      <c r="AA1" s="6"/>
-      <c r="AB1" s="6"/>
-      <c r="AC1" s="6"/>
-      <c r="AD1" s="6" t="s">
+      <c r="X1" s="19"/>
+      <c r="Y1" s="19"/>
+      <c r="Z1" s="19"/>
+      <c r="AA1" s="19"/>
+      <c r="AB1" s="19"/>
+      <c r="AC1" s="19"/>
+      <c r="AD1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="AE1" s="6"/>
-      <c r="AF1" s="6"/>
-      <c r="AG1" s="6"/>
-      <c r="AH1" s="6"/>
-      <c r="AI1" s="6"/>
-      <c r="AJ1" s="6"/>
-      <c r="AK1" s="6" t="s">
+      <c r="AE1" s="19"/>
+      <c r="AF1" s="19"/>
+      <c r="AG1" s="19"/>
+      <c r="AH1" s="19"/>
+      <c r="AI1" s="19"/>
+      <c r="AJ1" s="19"/>
+      <c r="AK1" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="AL1" s="6"/>
-      <c r="AM1" s="6"/>
-      <c r="AN1" s="6"/>
-      <c r="AO1" s="6"/>
-      <c r="AP1" s="6"/>
-      <c r="AQ1" s="6"/>
-      <c r="AR1" s="6" t="s">
+      <c r="AL1" s="19"/>
+      <c r="AM1" s="19"/>
+      <c r="AN1" s="19"/>
+      <c r="AO1" s="19"/>
+      <c r="AP1" s="19"/>
+      <c r="AQ1" s="19"/>
+      <c r="AR1" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="AS1" s="6"/>
-      <c r="AT1" s="6"/>
-      <c r="AU1" s="6"/>
-      <c r="AV1" s="6"/>
-      <c r="AW1" s="6"/>
-      <c r="AX1" s="6"/>
-      <c r="AY1" s="6" t="s">
+      <c r="AS1" s="19"/>
+      <c r="AT1" s="19"/>
+      <c r="AU1" s="19"/>
+      <c r="AV1" s="19"/>
+      <c r="AW1" s="19"/>
+      <c r="AX1" s="19"/>
+      <c r="AY1" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="AZ1" s="6"/>
-      <c r="BA1" s="6"/>
-      <c r="BB1" s="6"/>
-      <c r="BC1" s="6"/>
-      <c r="BD1" s="6"/>
-      <c r="BE1" s="6"/>
-      <c r="BF1" s="6" t="s">
+      <c r="AZ1" s="19"/>
+      <c r="BA1" s="19"/>
+      <c r="BB1" s="19"/>
+      <c r="BC1" s="19"/>
+      <c r="BD1" s="19"/>
+      <c r="BE1" s="19"/>
+      <c r="BF1" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="BG1" s="6"/>
-      <c r="BH1" s="6"/>
-      <c r="BI1" s="6"/>
-      <c r="BJ1" s="6"/>
-      <c r="BK1" s="6"/>
-      <c r="BL1" s="6"/>
-      <c r="BM1" s="6" t="s">
+      <c r="BG1" s="19"/>
+      <c r="BH1" s="19"/>
+      <c r="BI1" s="19"/>
+      <c r="BJ1" s="19"/>
+      <c r="BK1" s="19"/>
+      <c r="BL1" s="19"/>
+      <c r="BM1" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="BN1" s="6"/>
-      <c r="BO1" s="6"/>
-      <c r="BP1" s="6"/>
-      <c r="BQ1" s="6"/>
-      <c r="BR1" s="6"/>
-      <c r="BS1" s="6"/>
-      <c r="BT1" s="6" t="s">
+      <c r="BN1" s="19"/>
+      <c r="BO1" s="19"/>
+      <c r="BP1" s="19"/>
+      <c r="BQ1" s="19"/>
+      <c r="BR1" s="19"/>
+      <c r="BS1" s="19"/>
+      <c r="BT1" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="BU1" s="6"/>
-      <c r="BV1" s="6"/>
-      <c r="BW1" s="6"/>
-      <c r="BX1" s="6"/>
-      <c r="BY1" s="6"/>
-      <c r="BZ1" s="6"/>
-      <c r="CA1" s="6" t="s">
+      <c r="BU1" s="19"/>
+      <c r="BV1" s="19"/>
+      <c r="BW1" s="19"/>
+      <c r="BX1" s="19"/>
+      <c r="BY1" s="19"/>
+      <c r="BZ1" s="19"/>
+      <c r="CA1" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="CB1" s="6"/>
-      <c r="CC1" s="6"/>
-      <c r="CD1" s="6"/>
-      <c r="CE1" s="6"/>
+      <c r="CB1" s="19"/>
+      <c r="CC1" s="19"/>
+      <c r="CD1" s="19"/>
+      <c r="CE1" s="19"/>
     </row>
     <row r="2" spans="1:83" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
-      <c r="B2" s="7">
+      <c r="B2" s="6">
         <v>44319</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="6">
         <v>44320</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="6">
         <v>44321</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="6">
         <v>44322</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="6">
         <v>44323</v>
       </c>
-      <c r="G2" s="7">
+      <c r="G2" s="6">
         <v>44324</v>
       </c>
-      <c r="H2" s="7">
+      <c r="H2" s="6">
         <v>44325</v>
       </c>
-      <c r="I2" s="8">
+      <c r="I2" s="7">
         <v>44326</v>
       </c>
-      <c r="J2" s="8">
+      <c r="J2" s="7">
         <v>44327</v>
       </c>
-      <c r="K2" s="8">
+      <c r="K2" s="7">
         <v>44328</v>
       </c>
-      <c r="L2" s="8">
+      <c r="L2" s="7">
         <v>44329</v>
       </c>
-      <c r="M2" s="8">
+      <c r="M2" s="7">
         <v>44330</v>
       </c>
-      <c r="N2" s="8">
+      <c r="N2" s="7">
         <v>44331</v>
       </c>
-      <c r="O2" s="8">
+      <c r="O2" s="7">
         <v>44332</v>
       </c>
-      <c r="P2" s="9">
+      <c r="P2" s="8">
         <v>44333</v>
       </c>
-      <c r="Q2" s="9">
+      <c r="Q2" s="8">
         <v>44334</v>
       </c>
-      <c r="R2" s="9">
+      <c r="R2" s="8">
         <v>44335</v>
       </c>
-      <c r="S2" s="9">
+      <c r="S2" s="8">
         <v>44336</v>
       </c>
-      <c r="T2" s="9">
+      <c r="T2" s="8">
         <v>44337</v>
       </c>
-      <c r="U2" s="9">
+      <c r="U2" s="8">
         <v>44338</v>
       </c>
-      <c r="V2" s="9">
+      <c r="V2" s="8">
         <v>44339</v>
       </c>
-      <c r="W2" s="10">
+      <c r="W2" s="9">
         <v>44340</v>
       </c>
-      <c r="X2" s="10">
+      <c r="X2" s="9">
         <v>44341</v>
       </c>
-      <c r="Y2" s="10">
+      <c r="Y2" s="9">
         <v>44342</v>
       </c>
-      <c r="Z2" s="10">
+      <c r="Z2" s="9">
         <v>44343</v>
       </c>
-      <c r="AA2" s="10">
+      <c r="AA2" s="9">
         <v>44344</v>
       </c>
-      <c r="AB2" s="10">
+      <c r="AB2" s="9">
         <v>44345</v>
       </c>
-      <c r="AC2" s="10">
+      <c r="AC2" s="9">
         <v>44346</v>
       </c>
-      <c r="AD2" s="11">
+      <c r="AD2" s="10">
         <v>44347</v>
       </c>
-      <c r="AE2" s="11">
+      <c r="AE2" s="10">
         <v>44348</v>
       </c>
-      <c r="AF2" s="11">
+      <c r="AF2" s="10">
         <v>44349</v>
       </c>
-      <c r="AG2" s="11">
+      <c r="AG2" s="10">
         <v>44350</v>
       </c>
-      <c r="AH2" s="11">
+      <c r="AH2" s="10">
         <v>44351</v>
       </c>
-      <c r="AI2" s="11">
+      <c r="AI2" s="10">
         <v>44352</v>
       </c>
-      <c r="AJ2" s="11">
+      <c r="AJ2" s="10">
         <v>44353</v>
       </c>
-      <c r="AK2" s="12">
+      <c r="AK2" s="11">
         <v>44354</v>
       </c>
-      <c r="AL2" s="12">
+      <c r="AL2" s="11">
         <v>44355</v>
       </c>
-      <c r="AM2" s="12">
+      <c r="AM2" s="11">
         <v>44356</v>
       </c>
-      <c r="AN2" s="12">
+      <c r="AN2" s="11">
         <v>44357</v>
       </c>
-      <c r="AO2" s="12">
+      <c r="AO2" s="11">
         <v>44358</v>
       </c>
-      <c r="AP2" s="12">
+      <c r="AP2" s="11">
         <v>44359</v>
       </c>
-      <c r="AQ2" s="12">
+      <c r="AQ2" s="11">
         <v>44360</v>
       </c>
-      <c r="AR2" s="13">
+      <c r="AR2" s="12">
         <v>44361</v>
       </c>
-      <c r="AS2" s="13">
+      <c r="AS2" s="12">
         <v>44362</v>
       </c>
-      <c r="AT2" s="13">
+      <c r="AT2" s="12">
         <v>44363</v>
       </c>
-      <c r="AU2" s="13">
+      <c r="AU2" s="12">
         <v>44364</v>
       </c>
-      <c r="AV2" s="13">
+      <c r="AV2" s="12">
         <v>44365</v>
       </c>
-      <c r="AW2" s="13">
+      <c r="AW2" s="12">
         <v>44366</v>
       </c>
-      <c r="AX2" s="13">
+      <c r="AX2" s="12">
         <v>44367</v>
       </c>
-      <c r="AY2" s="14">
+      <c r="AY2" s="13">
         <v>44368</v>
       </c>
-      <c r="AZ2" s="14">
+      <c r="AZ2" s="13">
         <v>44369</v>
       </c>
-      <c r="BA2" s="14">
+      <c r="BA2" s="13">
         <v>44370</v>
       </c>
-      <c r="BB2" s="14">
+      <c r="BB2" s="13">
         <v>44371</v>
       </c>
-      <c r="BC2" s="14">
+      <c r="BC2" s="13">
         <v>44372</v>
       </c>
-      <c r="BD2" s="14">
+      <c r="BD2" s="13">
         <v>44373</v>
       </c>
-      <c r="BE2" s="14">
+      <c r="BE2" s="13">
         <v>44374</v>
       </c>
-      <c r="BF2" s="15">
+      <c r="BF2" s="14">
         <v>44375</v>
       </c>
-      <c r="BG2" s="15">
+      <c r="BG2" s="14">
         <v>44376</v>
       </c>
-      <c r="BH2" s="15">
+      <c r="BH2" s="14">
         <v>44377</v>
       </c>
-      <c r="BI2" s="15">
+      <c r="BI2" s="14">
         <v>44378</v>
       </c>
-      <c r="BJ2" s="15">
+      <c r="BJ2" s="14">
         <v>44379</v>
       </c>
-      <c r="BK2" s="15">
+      <c r="BK2" s="14">
         <v>44380</v>
       </c>
-      <c r="BL2" s="15">
+      <c r="BL2" s="14">
         <v>44381</v>
       </c>
-      <c r="BM2" s="16">
+      <c r="BM2" s="15">
         <v>44382</v>
       </c>
-      <c r="BN2" s="16">
+      <c r="BN2" s="15">
         <v>44383</v>
       </c>
-      <c r="BO2" s="16">
+      <c r="BO2" s="15">
         <v>44384</v>
       </c>
-      <c r="BP2" s="16">
+      <c r="BP2" s="15">
         <v>44385</v>
       </c>
-      <c r="BQ2" s="16">
+      <c r="BQ2" s="15">
         <v>44386</v>
       </c>
-      <c r="BR2" s="16">
+      <c r="BR2" s="15">
         <v>44387</v>
       </c>
-      <c r="BS2" s="16">
+      <c r="BS2" s="15">
         <v>44388</v>
       </c>
-      <c r="BT2" s="17">
+      <c r="BT2" s="16">
         <v>44389</v>
       </c>
-      <c r="BU2" s="17">
+      <c r="BU2" s="16">
         <v>44390</v>
       </c>
-      <c r="BV2" s="17">
+      <c r="BV2" s="16">
         <v>44391</v>
       </c>
-      <c r="BW2" s="17">
+      <c r="BW2" s="16">
         <v>44392</v>
       </c>
-      <c r="BX2" s="17">
+      <c r="BX2" s="16">
         <v>44393</v>
       </c>
-      <c r="BY2" s="17">
+      <c r="BY2" s="16">
         <v>44394</v>
       </c>
-      <c r="BZ2" s="17">
+      <c r="BZ2" s="16">
         <v>44395</v>
       </c>
-      <c r="CA2" s="18">
+      <c r="CA2" s="17">
         <v>44396</v>
       </c>
-      <c r="CB2" s="18">
+      <c r="CB2" s="17">
         <v>44397</v>
       </c>
-      <c r="CC2" s="18">
+      <c r="CC2" s="17">
         <v>44398</v>
       </c>
-      <c r="CD2" s="18">
+      <c r="CD2" s="17">
         <v>44399</v>
       </c>
-      <c r="CE2" s="18">
+      <c r="CE2" s="17">
         <v>44400</v>
       </c>
     </row>
     <row r="3" spans="1:83" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -1157,7 +1155,7 @@
     </row>
     <row r="5" spans="1:83" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -1329,7 +1327,7 @@
     </row>
     <row r="7" spans="1:83" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -1501,7 +1499,7 @@
     </row>
     <row r="9" spans="1:83" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -1673,7 +1671,7 @@
     </row>
     <row r="11" spans="1:83" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -1845,7 +1843,7 @@
     </row>
     <row r="13" spans="1:83" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -2017,7 +2015,7 @@
     </row>
     <row r="15" spans="1:83" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -2189,7 +2187,7 @@
     </row>
     <row r="17" spans="1:83" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -2360,27 +2358,22 @@
       <c r="CE18" s="4"/>
     </row>
     <row r="20" spans="1:83" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="19"/>
+      <c r="B20" s="18"/>
     </row>
     <row r="21" spans="1:83" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B21" s="3"/>
     </row>
     <row r="22" spans="1:83" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B22" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="AR1:AX1"/>
-    <mergeCell ref="AY1:BE1"/>
-    <mergeCell ref="BF1:BL1"/>
-    <mergeCell ref="BM1:BS1"/>
-    <mergeCell ref="BT1:BZ1"/>
     <mergeCell ref="CA1:CE1"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="I1:O1"/>
@@ -2388,6 +2381,11 @@
     <mergeCell ref="W1:AC1"/>
     <mergeCell ref="AD1:AJ1"/>
     <mergeCell ref="AK1:AQ1"/>
+    <mergeCell ref="AR1:AX1"/>
+    <mergeCell ref="AY1:BE1"/>
+    <mergeCell ref="BF1:BL1"/>
+    <mergeCell ref="BM1:BS1"/>
+    <mergeCell ref="BT1:BZ1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>